<commit_message>
showall and add product finished
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -25,13 +25,34 @@
     <t>PhPrice</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>fffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffff</t>
+  </si>
+  <si>
     <t>testname</t>
   </si>
   <si>
+    <t>tt</t>
+  </si>
+  <si>
+    <t>zzzz</t>
+  </si>
+  <si>
     <t>تجربة</t>
-  </si>
-  <si>
-    <t>tt</t>
   </si>
 </sst>
 </file>
@@ -389,7 +410,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,10 +435,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -428,10 +449,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>15.5</v>
+        <v>5.5</v>
       </c>
       <c r="D3">
-        <v>20.25</v>
+        <v>6.7</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -442,10 +463,108 @@
         <v>5</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>5.7</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
         <v>10.025</v>
       </c>
-      <c r="D4">
+      <c r="D9">
         <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit and remove finished
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -28,28 +28,13 @@
     <t>a</t>
   </si>
   <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>d</t>
   </si>
   <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>fffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffff</t>
+    <t>ffffffffffffffffffffffffffffffffffffffffffffffffffffffffffffff</t>
   </si>
   <si>
     <t>g</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>i</t>
   </si>
   <si>
     <t>testname</t>
@@ -419,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,10 +429,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -458,10 +443,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>5.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>6.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -472,7 +457,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -500,10 +485,10 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>5.7</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -514,10 +499,10 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>10.025</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -528,10 +513,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.01</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -542,79 +527,9 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12">
-        <v>10.025</v>
-      </c>
-      <c r="D12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
         <v>2</v>
       </c>
     </row>

</xml_diff>